<commit_message>
made changes to annotations
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -15,33 +15,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>900.0</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+  <si>
+    <t>5.5 GHz</t>
+  </si>
+  <si>
+    <t>5500.0</t>
+  </si>
+  <si>
+    <t>1000.0</t>
+  </si>
+  <si>
+    <t>5000.0</t>
+  </si>
+  <si>
+    <t>6000.0</t>
+  </si>
+  <si>
+    <t>0.1571</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>-50</t>
+  </si>
+  <si>
+    <t>4 GHz</t>
+  </si>
+  <si>
+    <t>4000.0</t>
+  </si>
+  <si>
+    <t>3500.0</t>
+  </si>
+  <si>
+    <t>4500.0</t>
+  </si>
+  <si>
+    <t>915 MHz</t>
+  </si>
+  <si>
+    <t>915.0</t>
   </si>
   <si>
     <t>100.0</t>
   </si>
   <si>
-    <t>850.0</t>
-  </si>
-  <si>
-    <t>950.0</t>
-  </si>
-  <si>
-    <t>315.0</t>
+    <t>865.0</t>
+  </si>
+  <si>
+    <t>965.0</t>
+  </si>
+  <si>
+    <t>0.03945</t>
+  </si>
+  <si>
+    <t>863 MHz</t>
+  </si>
+  <si>
+    <t>863.0</t>
+  </si>
+  <si>
+    <t>813.0</t>
+  </si>
+  <si>
+    <t>913.0</t>
+  </si>
+  <si>
+    <t>Wide Band</t>
+  </si>
+  <si>
+    <t>3015.0</t>
+  </si>
+  <si>
+    <t>5970.0</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>0.3156</t>
   </si>
   <si>
     <t>1.0</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>-65</t>
   </si>
 </sst>
 </file>
@@ -377,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -411,6 +471,122 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>